<commit_message>
Added sensors to RoboRIO Ports file
</commit_message>
<xml_diff>
--- a/RoboRIO Ports.xlsx
+++ b/RoboRIO Ports.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Port</t>
   </si>
@@ -102,6 +102,30 @@
   </si>
   <si>
     <t>Scaler Right Lift</t>
+  </si>
+  <si>
+    <t>DIO 0/1</t>
+  </si>
+  <si>
+    <t>Left Wheel Encoder</t>
+  </si>
+  <si>
+    <t>DIO 2/3</t>
+  </si>
+  <si>
+    <t>Right Wheel Encoder</t>
+  </si>
+  <si>
+    <t>Analog In 0</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>Beam Break Sensor</t>
+  </si>
+  <si>
+    <t>DIO 4/5</t>
   </si>
 </sst>
 </file>
@@ -432,14 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -539,6 +564,38 @@
       </c>
       <c r="C9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>